<commit_message>
Switched labels for 8A and 8B so that they are in chronological order
</commit_message>
<xml_diff>
--- a/data/mic_mic2.xlsx
+++ b/data/mic_mic2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bjpessman/Documents/phd_research_code/Vibratory_Noise/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91BC5972-4530-5D41-B74C-B46B00BD466E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525DF609-EA3C-F04F-A8D4-45E4F02A9111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="26780" windowHeight="15940" xr2:uid="{F34ACBF8-4A74-AB47-9F15-6287E73A142A}"/>
   </bookViews>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC794D48-80DC-144B-AE41-63FAFA448EA2}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1674,7 +1674,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B86" t="s">
         <v>25</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B87" t="s">
         <v>25</v>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B88" t="s">
         <v>26</v>
@@ -1716,7 +1716,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B89" t="s">
         <v>26</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B90" t="s">
         <v>25</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B91" t="s">
         <v>25</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B92" t="s">
         <v>26</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B93" t="s">
         <v>26</v>

</xml_diff>